<commit_message>
added new lists download
</commit_message>
<xml_diff>
--- a/downloads/KB-Liste Red Holstein.xlsx
+++ b/downloads/KB-Liste Red Holstein.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Anna\HP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F38FE26-03B5-4B03-A754-858C6F75338E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8247BB92-FA2E-4AA1-9A09-5C52C2FADE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{753348B5-95AC-4BE2-93B4-742E884FAC32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{753348B5-95AC-4BE2-93B4-742E884FAC32}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="127">
   <si>
     <t>Red Holstein et al. SVKB</t>
   </si>
@@ -443,13 +443,60 @@
     <t>* = CDH-Träger, nicht an CDH-Trägerin! Trägerin in Besamerkarte markiert</t>
   </si>
   <si>
-    <t>Inhalt, Euter, Nutzungsdau</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +1627, Inhalt, Nutzungsdauer</t>
-  </si>
-  <si>
-    <t>Sunboy-ET</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sunboy-ET</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Prüf)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Inhalt, Euter, Nutzungsdau </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(nicht 004/005)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> +1627, Inhalt, Nutzungsdau </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(nicht 011/012)</t>
+    </r>
+  </si>
+  <si>
+    <t>X-SUV PP</t>
+  </si>
+  <si>
+    <t>67 o</t>
+  </si>
+  <si>
+    <t>Roboter, Geburt, ZZ, Fruchtbar, Exterieur</t>
   </si>
 </sst>
 </file>
@@ -622,7 +669,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -709,7 +756,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1026,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB452BD-4C3A-43F3-BEE9-72D3A9834308}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1095,7 @@
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1">
-        <v>44382</v>
+        <v>44407</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
@@ -1631,8 +1677,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
-        <v>123</v>
+      <c r="A32" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>8</v>
@@ -1748,9 +1794,7 @@
       <c r="C38" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>101</v>
-      </c>
+      <c r="D38" s="12"/>
       <c r="E38" s="2" t="s">
         <v>21</v>
       </c>
@@ -1772,7 +1816,7 @@
         <v>101</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F39" s="31">
         <v>108</v>
@@ -1812,7 +1856,7 @@
         <v>101</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F41" s="31">
         <v>89</v>
@@ -1900,46 +1944,66 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="B46" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="33" t="s">
+      <c r="B47" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="2" t="s">
+      <c r="D47" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F46" s="28" t="s">
+      <c r="F47" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="36"/>
-    </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="35"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="36"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="41"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A49:F49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>